<commit_message>
Add function and pages
Realize the function of generate chart using AI. Realize limiting usage of the user.
Add relevant frontend pages.
</commit_message>
<xml_diff>
--- a/EasyBI-backend/src/main/resources/test_excel.xlsx
+++ b/EasyBI-backend/src/main/resources/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS\project\bi\EasyBI\EasyBI-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4252FA-1078-494A-A778-BA714D1A3299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26567E0-351D-41F0-BB7B-501B90583F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="2550" windowWidth="18910" windowHeight="12130" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
   </bookViews>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260829AF-83D5-9D43-A57C-13A2BDCFFDE0}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="22.5"/>
@@ -477,6 +477,30 @@
         <v>30</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>